<commit_message>
PECAS SR13 release setup. (PECAS-79) (PECAS-80) (PECAS-81)
</commit_message>
<xml_diff>
--- a/docs/DPbyDLambdaCheck.xlsx
+++ b/docs/DPbyDLambdaCheck.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="34395" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -56,8 +56,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -65,6 +65,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,6 +96,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,16 +423,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -434,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -450,7 +456,7 @@
         <v>0.40175957853335542</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -466,7 +472,7 @@
         <v>0.32893292228890675</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -482,7 +488,7 @@
         <v>0.26930749917773789</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -490,7 +496,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8">
         <f>SUM(C3:C5)</f>
         <v>6.7659415573420221</v>
@@ -500,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>4</v>
       </c>
@@ -508,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -524,7 +530,7 @@
         <v>0.40176306399221595</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -540,7 +546,7 @@
         <v>0.32893248659995172</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -556,7 +562,7 @@
         <v>0.26930444940783232</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -564,7 +570,7 @@
         <v>0.20000999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C19">
         <f>SUM(C14:C16)</f>
         <v>6.7662211626329229</v>
@@ -574,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -583,19 +589,19 @@
         <v>0.34854588605366099</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24">
         <f>(D15-D4)/($B$17-$B$6)</f>
         <v>-4.3568895502576671E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D25">
         <f>(D16-D5)/($B$17-$B$6)</f>
         <v>-0.30497699055663541</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -604,17 +610,22 @@
         <v>0.34854608514462998</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29">
         <f>D15*(B15*(D14+D16)-B14*D14-B16*D16)</f>
         <v>-4.3569941466825843E-2</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f>D16*(B16*(D14+D15)-B14*D14-B15*D15)</f>
+        <v>-0.30497614367780396</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>